<commit_message>
sort and sum up two brand sheets.
</commit_message>
<xml_diff>
--- a/sample2.xlsx
+++ b/sample2.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maggie/Documents/CS/Python/tp-weekppt/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A4CF66-ABB2-9A46-872B-0CBD6CF36B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -52,9 +58,6 @@
     <t>B0CSFP3THQ</t>
   </si>
   <si>
-    <t>TMP-140L</t>
-  </si>
-  <si>
     <t>-34.12%</t>
   </si>
   <si>
@@ -119,16 +122,19 @@
   </si>
   <si>
     <t>B097MDK93V</t>
+  </si>
+  <si>
+    <t>TPM-140L</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.00;-#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00;\-#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,26 +193,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +261,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -278,6 +295,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,9 +330,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,28 +506,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="1" max="5" width="20.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -525,7 +546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8" customHeight="1">
+    <row r="3" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -542,7 +563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8" customHeight="1">
+    <row r="4" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -550,160 +571,157 @@
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3">
         <v>-108.49</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="3">
         <v>-53.45</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1"/>
       <c r="D6" s="3">
         <v>-7.47</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="3">
         <v>-14.81</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>-172.9</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="3">
         <v>-175.86</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D10" s="3">
         <v>-33.14</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="16.8" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D11" s="3">
         <v>-22.31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16.8" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="1"/>
+        <v>32</v>
+      </c>
       <c r="D12" s="3">
         <v>-5.08</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="16.8" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="1"/>
+        <v>33</v>
+      </c>
       <c r="D13" s="3">
         <v>-4.42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>